<commit_message>
Das hier ist der Aktuellster Stand (27.11.2023)
</commit_message>
<xml_diff>
--- a/Dokumentation/Kopie von Auto_ESY_Stand_22_11.xlsx
+++ b/Dokumentation/Kopie von Auto_ESY_Stand_22_11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blagoje\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Gruppe_05\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41B47F5-285C-4B2E-A963-B6B986B1C286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918A578F-13E8-49B1-A99D-50678DA7DD90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" tabRatio="500" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -42,17 +42,6 @@
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -1853,6 +1842,30 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1871,32 +1884,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2058,7 +2047,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Stammdaten"/>
@@ -2396,27 +2385,27 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="5" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="5" customWidth="1"/>
-    <col min="5" max="6" width="19.26953125" style="5" customWidth="1"/>
-    <col min="7" max="1024" width="11.453125" style="5"/>
+    <col min="2" max="2" width="22.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="5" customWidth="1"/>
+    <col min="5" max="6" width="19.28515625" style="5" customWidth="1"/>
+    <col min="7" max="1024" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="119" t="s">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2433,7 +2422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -2450,7 +2439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2463,12 +2452,12 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="114" t="s">
+      <c r="E7" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="114"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="109"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
@@ -2477,45 +2466,45 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="121"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>17</v>
       </c>
@@ -2525,55 +2514,55 @@
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="117"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="114"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="115"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="115"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="115"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="115"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="115"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="112"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>22</v>
       </c>
@@ -2583,75 +2572,65 @@
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="113" t="s">
+    <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="113"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="113"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="121"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="121"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="114" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="114"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="114" t="s">
+      <c r="B26" s="109"/>
+      <c r="C26" s="109"/>
+      <c r="D26" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
-    </row>
-    <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="109" t="s">
+      <c r="E26" s="109"/>
+      <c r="F26" s="109"/>
+    </row>
+    <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="109"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
-    </row>
-    <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="108" t="s">
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+    </row>
+    <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="108"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109" t="s">
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="117" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="109"/>
-      <c r="F28" s="109"/>
-    </row>
-    <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="110" t="s">
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+    </row>
+    <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="110"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="111"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2662,6 +2641,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2677,14 +2666,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" style="100" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" style="100" customWidth="1"/>
-    <col min="3" max="1024" width="11.54296875" style="100"/>
+    <col min="1" max="1" width="13.28515625" style="100" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="100" customWidth="1"/>
+    <col min="3" max="1024" width="11.5703125" style="100"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>198</v>
       </c>
@@ -2692,7 +2681,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
         <v>200</v>
       </c>
@@ -2700,7 +2689,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="100" t="s">
         <v>202</v>
       </c>
@@ -2725,41 +2714,41 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
-    <col min="2" max="2" width="58.81640625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="39.54296875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="64" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="64" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="119" t="s">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-    </row>
-    <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+    </row>
+    <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="123" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="123"/>
     </row>
-    <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="123" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="123"/>
     </row>
-    <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="123" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="123"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>33</v>
       </c>
@@ -2773,7 +2762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>10</v>
       </c>
@@ -2785,7 +2774,7 @@
       </c>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="28">
         <v>20</v>
       </c>
@@ -2797,7 +2786,7 @@
       </c>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>30</v>
       </c>
@@ -2809,7 +2798,7 @@
       </c>
       <c r="D11" s="30"/>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>40</v>
       </c>
@@ -2821,7 +2810,7 @@
       </c>
       <c r="D12" s="30"/>
     </row>
-    <row r="13" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>51</v>
       </c>
@@ -2833,7 +2822,7 @@
       </c>
       <c r="D13" s="30"/>
     </row>
-    <row r="14" spans="1:4" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="28">
         <v>52</v>
       </c>
@@ -2845,13 +2834,13 @@
       </c>
       <c r="D14" s="30"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="29"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="28">
         <v>60</v>
       </c>
@@ -2863,7 +2852,7 @@
       </c>
       <c r="D16" s="30"/>
     </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>61</v>
       </c>
@@ -2875,7 +2864,7 @@
       </c>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
         <v>62</v>
       </c>
@@ -2887,7 +2876,7 @@
       </c>
       <c r="D18" s="30"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
         <v>50</v>
       </c>
@@ -2895,7 +2884,7 @@
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="28">
         <v>60</v>
       </c>
@@ -2903,7 +2892,7 @@
       <c r="C20" s="30"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="28">
         <v>70</v>
       </c>
@@ -2911,7 +2900,7 @@
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="28">
         <v>80</v>
       </c>
@@ -2919,7 +2908,7 @@
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="28">
         <v>90</v>
       </c>
@@ -2927,7 +2916,7 @@
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="28">
         <v>100</v>
       </c>
@@ -2935,7 +2924,7 @@
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="32">
         <v>110</v>
       </c>
@@ -2943,7 +2932,7 @@
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2972,45 +2961,45 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.453125" customWidth="1"/>
-    <col min="2" max="3" width="11.7265625" customWidth="1"/>
-    <col min="4" max="64" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="64" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="124" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="124"/>
       <c r="C1" s="124"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
       <c r="B2" s="35"/>
       <c r="C2" s="23"/>
     </row>
-    <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="125" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="125"/>
       <c r="C3" s="125"/>
     </row>
-    <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="126" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="126"/>
       <c r="C4" s="126"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>55</v>
       </c>
@@ -3021,7 +3010,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -3032,7 +3021,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>59</v>
       </c>
@@ -3043,7 +3032,7 @@
         <v>45243</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>209</v>
       </c>
@@ -3054,7 +3043,7 @@
         <v>45250</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
@@ -3063,7 +3052,7 @@
       </c>
       <c r="C10" s="41"/>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -3072,7 +3061,7 @@
       </c>
       <c r="C11" s="41"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
@@ -3081,7 +3070,7 @@
       </c>
       <c r="C12" s="41"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>63</v>
       </c>
@@ -3090,7 +3079,7 @@
       </c>
       <c r="C13" s="41"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -3099,7 +3088,7 @@
       </c>
       <c r="C14" s="41"/>
     </row>
-    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -3108,7 +3097,7 @@
       </c>
       <c r="C15" s="41"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
@@ -3117,126 +3106,126 @@
       </c>
       <c r="C16" s="41"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="40"/>
       <c r="C18" s="41"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="40"/>
       <c r="C21" s="41"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="40"/>
       <c r="C24" s="41"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="41"/>
       <c r="C31" s="41"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="41"/>
       <c r="C32" s="41"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="41"/>
       <c r="C33" s="41"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="41"/>
       <c r="C34" s="41"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="41"/>
       <c r="C36" s="41"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="41"/>
       <c r="C37" s="41"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="41"/>
       <c r="C38" s="41"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="41"/>
       <c r="C39" s="41"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="41"/>
       <c r="C40" s="41"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="42"/>
       <c r="C41" s="42"/>
@@ -3263,18 +3252,18 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.453125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="43.81640625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="68.7265625" style="23" customWidth="1"/>
-    <col min="7" max="1024" width="11.453125" style="23"/>
+    <col min="1" max="1" width="3.42578125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="68.7109375" style="23" customWidth="1"/>
+    <col min="7" max="1024" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="124" t="s">
         <v>67</v>
       </c>
@@ -3284,7 +3273,7 @@
       <c r="E1" s="124"/>
       <c r="F1" s="124"/>
     </row>
-    <row r="3" spans="1:6" s="43" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -3304,7 +3293,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="41">
         <v>1</v>
       </c>
@@ -3322,7 +3311,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="41">
         <v>2</v>
       </c>
@@ -3340,7 +3329,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
         <v>3</v>
       </c>
@@ -3356,7 +3345,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="45"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
         <v>4</v>
       </c>
@@ -3371,7 +3360,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
         <v>5</v>
       </c>
@@ -3389,7 +3378,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="41">
         <v>6</v>
       </c>
@@ -3407,7 +3396,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="41">
         <v>9</v>
       </c>
@@ -3423,7 +3412,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>10</v>
       </c>
@@ -3439,7 +3428,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="46"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>11</v>
       </c>
@@ -3449,7 +3438,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="41">
         <v>12</v>
       </c>
@@ -3459,7 +3448,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="41">
         <v>13</v>
       </c>
@@ -3469,7 +3458,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>14</v>
       </c>
@@ -3479,7 +3468,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="41">
         <v>26</v>
       </c>
@@ -3489,7 +3478,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="41">
         <v>27</v>
       </c>
@@ -3499,7 +3488,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="41">
         <v>28</v>
       </c>
@@ -3509,7 +3498,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="41">
         <v>29</v>
       </c>
@@ -3519,7 +3508,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>30</v>
       </c>
@@ -3529,7 +3518,7 @@
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
     </row>
-    <row r="21" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="43" t="s">
         <v>85</v>
@@ -3564,29 +3553,29 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
-    <col min="2" max="2" width="65.81640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="49" customWidth="1"/>
-    <col min="4" max="6" width="13.7265625" style="49" customWidth="1"/>
-    <col min="7" max="8" width="14.453125" style="49" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="65.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="49" customWidth="1"/>
+    <col min="4" max="6" width="13.7109375" style="49" customWidth="1"/>
+    <col min="7" max="8" width="14.42578125" style="49" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="119" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-    </row>
-    <row r="3" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+    </row>
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -3615,7 +3604,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="51">
         <v>10</v>
       </c>
@@ -3630,7 +3619,7 @@
       <c r="H4" s="53"/>
       <c r="I4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>11</v>
       </c>
@@ -3653,7 +3642,7 @@
       <c r="H5" s="58"/>
       <c r="I5" s="59"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>12</v>
       </c>
@@ -3682,7 +3671,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>13</v>
       </c>
@@ -3711,7 +3700,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>14</v>
       </c>
@@ -3726,7 +3715,7 @@
       <c r="H8" s="58"/>
       <c r="I8" s="59"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="28"/>
       <c r="B9" s="55"/>
       <c r="C9" s="56"/>
@@ -3737,7 +3726,7 @@
       <c r="H9" s="56"/>
       <c r="I9" s="59"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="60">
         <v>20</v>
       </c>
@@ -3752,7 +3741,7 @@
       <c r="H10" s="56"/>
       <c r="I10" s="59"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>21</v>
       </c>
@@ -3779,7 +3768,7 @@
       </c>
       <c r="I11" s="59"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>22</v>
       </c>
@@ -3806,7 +3795,7 @@
       </c>
       <c r="I12" s="59"/>
     </row>
-    <row r="13" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>23</v>
       </c>
@@ -3833,7 +3822,7 @@
       </c>
       <c r="I13" s="59"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="28">
         <v>24</v>
       </c>
@@ -3860,7 +3849,7 @@
       </c>
       <c r="I14" s="59"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="55"/>
       <c r="C15" s="56"/>
@@ -3871,7 +3860,7 @@
       <c r="H15" s="56"/>
       <c r="I15" s="59"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="60">
         <v>30</v>
       </c>
@@ -3886,7 +3875,7 @@
       <c r="H16" s="56"/>
       <c r="I16" s="59"/>
     </row>
-    <row r="17" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>31</v>
       </c>
@@ -3913,7 +3902,7 @@
       </c>
       <c r="I17" s="59"/>
     </row>
-    <row r="18" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
         <v>32</v>
       </c>
@@ -3940,7 +3929,7 @@
       </c>
       <c r="I18" s="59"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
         <v>34</v>
       </c>
@@ -3967,7 +3956,7 @@
       </c>
       <c r="I19" s="59"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="28">
         <v>35</v>
       </c>
@@ -3988,7 +3977,7 @@
       <c r="H20" s="56"/>
       <c r="I20" s="59"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="55"/>
       <c r="C21" s="56"/>
@@ -3999,7 +3988,7 @@
       <c r="H21" s="56"/>
       <c r="I21" s="59"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="60">
         <v>40</v>
       </c>
@@ -4014,7 +4003,7 @@
       <c r="H22" s="56"/>
       <c r="I22" s="59"/>
     </row>
-    <row r="23" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="61">
         <v>41</v>
       </c>
@@ -4035,7 +4024,7 @@
       <c r="H23" s="62"/>
       <c r="I23" s="63"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="61">
         <v>42</v>
       </c>
@@ -4056,7 +4045,7 @@
       <c r="H24" s="62"/>
       <c r="I24" s="63"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="61">
         <v>43</v>
       </c>
@@ -4077,7 +4066,7 @@
       <c r="H25" s="62"/>
       <c r="I25" s="63"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="61">
         <v>44</v>
       </c>
@@ -4098,7 +4087,7 @@
       <c r="H26" s="62"/>
       <c r="I26" s="63"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="61">
         <v>45</v>
       </c>
@@ -4119,7 +4108,7 @@
       <c r="H27" s="62"/>
       <c r="I27" s="63"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="61">
         <v>46</v>
       </c>
@@ -4142,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="28">
         <v>47</v>
       </c>
@@ -4163,7 +4152,7 @@
       <c r="H29" s="56"/>
       <c r="I29" s="59"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <v>48</v>
       </c>
@@ -4184,7 +4173,7 @@
       <c r="H30" s="56"/>
       <c r="I30" s="59"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="61"/>
       <c r="B31" s="64"/>
       <c r="C31" s="62"/>
@@ -4195,7 +4184,7 @@
       <c r="H31" s="62"/>
       <c r="I31" s="63"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="61"/>
       <c r="B32" s="64"/>
       <c r="C32" s="62"/>
@@ -4206,7 +4195,7 @@
       <c r="H32" s="62"/>
       <c r="I32" s="63"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="62"/>
@@ -4217,7 +4206,7 @@
       <c r="H33" s="62"/>
       <c r="I33" s="63"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
       <c r="B34" s="65"/>
       <c r="C34" s="66"/>
@@ -4228,7 +4217,7 @@
       <c r="H34" s="66"/>
       <c r="I34" s="67"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="49">
         <f>SUM(D10:D34)</f>
         <v>20</v>
@@ -4243,7 +4232,7 @@
       </c>
       <c r="I35" s="68"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I36" s="68"/>
     </row>
   </sheetData>
@@ -4268,23 +4257,23 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="13" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" style="69" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" style="69" customWidth="1"/>
-    <col min="10" max="10" width="38.7265625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="20.1796875" style="5" customWidth="1"/>
-    <col min="12" max="1024" width="11.453125" style="5"/>
+    <col min="4" max="4" width="11.140625" style="69" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="69" customWidth="1"/>
+    <col min="10" max="10" width="38.7109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="5" customWidth="1"/>
+    <col min="12" max="1024" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="127" t="s">
         <v>118</v>
       </c>
@@ -4299,7 +4288,7 @@
       <c r="J1" s="127"/>
       <c r="K1" s="127"/>
     </row>
-    <row r="3" spans="1:11" ht="26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
         <v>33</v>
       </c>
@@ -4334,7 +4323,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="72">
         <f t="shared" ref="A4:A33" si="0">ROW()-3</f>
         <v>1</v>
@@ -4366,7 +4355,7 @@
       <c r="J4" s="38"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4398,7 +4387,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="81"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4430,7 +4419,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="81"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4446,7 +4435,7 @@
       <c r="J7" s="81"/>
       <c r="K7" s="81"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4462,7 +4451,7 @@
       <c r="J8" s="81"/>
       <c r="K8" s="81"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="77">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4478,7 +4467,7 @@
       <c r="J9" s="81"/>
       <c r="K9" s="81"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="77">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4494,7 +4483,7 @@
       <c r="J10" s="81"/>
       <c r="K10" s="79"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="77">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4510,7 +4499,7 @@
       <c r="J11" s="81"/>
       <c r="K11" s="79"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="77">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4526,7 +4515,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="79"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="77">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4542,7 +4531,7 @@
       <c r="J13" s="81"/>
       <c r="K13" s="79"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="77">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4558,7 +4547,7 @@
       <c r="J14" s="81"/>
       <c r="K14" s="81"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="77">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4574,7 +4563,7 @@
       <c r="J15" s="81"/>
       <c r="K15" s="79"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="77">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4590,7 +4579,7 @@
       <c r="J16" s="81"/>
       <c r="K16" s="79"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="77">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4606,7 +4595,7 @@
       <c r="J17" s="81"/>
       <c r="K17" s="79"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="77">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4622,7 +4611,7 @@
       <c r="J18" s="79"/>
       <c r="K18" s="79"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="77">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4638,7 +4627,7 @@
       <c r="J19" s="81"/>
       <c r="K19" s="79"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="77">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4654,7 +4643,7 @@
       <c r="J20" s="81"/>
       <c r="K20" s="79"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="77">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4670,7 +4659,7 @@
       <c r="J21" s="81"/>
       <c r="K21" s="79"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="77">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4686,7 +4675,7 @@
       <c r="J22" s="81"/>
       <c r="K22" s="79"/>
     </row>
-    <row r="23" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="77">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4702,7 +4691,7 @@
       <c r="J23" s="81"/>
       <c r="K23" s="79"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="77">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4718,7 +4707,7 @@
       <c r="J24" s="81"/>
       <c r="K24" s="79"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="77">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4734,7 +4723,7 @@
       <c r="J25" s="81"/>
       <c r="K25" s="79"/>
     </row>
-    <row r="26" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="77">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4750,7 +4739,7 @@
       <c r="J26" s="81"/>
       <c r="K26" s="79"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="77">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4766,7 +4755,7 @@
       <c r="J27" s="81"/>
       <c r="K27" s="79"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="77">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4782,7 +4771,7 @@
       <c r="J28" s="81"/>
       <c r="K28" s="79"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="77">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4798,7 +4787,7 @@
       <c r="J29" s="81"/>
       <c r="K29" s="79"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="77">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4814,7 +4803,7 @@
       <c r="J30" s="81"/>
       <c r="K30" s="79"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="77">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4830,7 +4819,7 @@
       <c r="J31" s="81"/>
       <c r="K31" s="79"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="77">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4846,7 +4835,7 @@
       <c r="J32" s="81"/>
       <c r="K32" s="79"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="83">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4862,7 +4851,7 @@
       <c r="J33" s="87"/>
       <c r="K33" s="84"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="49"/>
       <c r="C34" s="88"/>
       <c r="E34" s="89"/>
@@ -4872,7 +4861,7 @@
       <c r="J34" s="90"/>
       <c r="K34" s="88"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="49"/>
       <c r="C35" s="88"/>
       <c r="E35" s="89"/>
@@ -4882,7 +4871,7 @@
       <c r="J35" s="90"/>
       <c r="K35" s="88"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>138</v>
       </c>
@@ -4893,7 +4882,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>140</v>
       </c>
@@ -4904,7 +4893,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>141</v>
       </c>
@@ -4915,15 +4904,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G39" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E45" s="91"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51" s="23"/>
     </row>
   </sheetData>
@@ -4949,18 +4938,18 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="23" customWidth="1"/>
     <col min="2" max="2" width="55" style="23" customWidth="1"/>
-    <col min="3" max="5" width="4.81640625" style="35" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" style="23" customWidth="1"/>
-    <col min="7" max="7" width="59.453125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="23" customWidth="1"/>
-    <col min="9" max="1024" width="11.453125" style="23"/>
+    <col min="3" max="5" width="4.85546875" style="35" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="59.42578125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="23" customWidth="1"/>
+    <col min="9" max="1024" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="124" t="s">
         <v>144</v>
       </c>
@@ -4972,10 +4961,10 @@
       <c r="G1" s="124"/>
       <c r="H1" s="124"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
     </row>
-    <row r="3" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -5001,7 +4990,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -5024,7 +5013,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -5047,7 +5036,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -5070,7 +5059,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -5085,7 +5074,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -5100,7 +5089,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -5115,7 +5104,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -5130,7 +5119,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -5145,7 +5134,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -5160,7 +5149,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -5175,7 +5164,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -5190,7 +5179,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -5205,7 +5194,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -5220,7 +5209,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -5235,7 +5224,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -5250,7 +5239,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -5265,7 +5254,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -5280,7 +5269,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -5295,7 +5284,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -5310,7 +5299,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -5325,7 +5314,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -5340,7 +5329,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -5355,7 +5344,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -5370,7 +5359,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -5385,7 +5374,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -5400,7 +5389,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -5415,7 +5404,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -5430,7 +5419,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -5445,7 +5434,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -5460,7 +5449,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="24">
         <v>30</v>
       </c>
@@ -5505,31 +5494,31 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="13" width="10.54296875" customWidth="1"/>
-    <col min="14" max="14" width="40.54296875" customWidth="1"/>
-    <col min="15" max="64" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="40.5703125" customWidth="1"/>
+    <col min="15" max="64" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="92" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="93" t="s">
         <v>160</v>
       </c>
@@ -5543,7 +5532,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="95" t="s">
         <v>164</v>
       </c>
@@ -5557,7 +5546,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="95" t="s">
         <v>168</v>
       </c>
@@ -5574,7 +5563,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="95" t="s">
         <v>172</v>
       </c>
@@ -5600,7 +5589,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="95" t="s">
         <v>179</v>
       </c>
@@ -5626,7 +5615,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="95" t="s">
         <v>183</v>
       </c>
@@ -5646,7 +5635,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="95"/>
       <c r="B10" s="96"/>
       <c r="C10" s="96"/>
@@ -5664,7 +5653,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="95"/>
       <c r="B11" s="96"/>
       <c r="C11" s="96"/>
@@ -5682,7 +5671,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="95"/>
       <c r="B12" s="96"/>
       <c r="C12" s="96"/>
@@ -5700,49 +5689,49 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="95"/>
       <c r="B13" s="96"/>
       <c r="C13" s="96"/>
       <c r="D13" s="96"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="95"/>
       <c r="B14" s="96"/>
       <c r="C14" s="96"/>
       <c r="D14" s="96"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="95"/>
       <c r="B15" s="96"/>
       <c r="C15" s="96"/>
       <c r="D15" s="96"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="95"/>
       <c r="B16" s="96"/>
       <c r="C16" s="96"/>
       <c r="D16" s="96"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="95"/>
       <c r="B17" s="96"/>
       <c r="C17" s="96"/>
       <c r="D17" s="96"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="95"/>
       <c r="B18" s="96"/>
       <c r="C18" s="96"/>
       <c r="D18" s="96"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="95"/>
       <c r="B19" s="96"/>
       <c r="C19" s="96"/>
       <c r="D19" s="96"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="93" t="s">
         <v>160</v>
       </c>
@@ -5752,7 +5741,7 @@
       <c r="C21" s="129"/>
       <c r="D21" s="129"/>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="98" t="s">
         <v>179</v>
       </c>
@@ -5762,7 +5751,7 @@
       <c r="C22" s="130"/>
       <c r="D22" s="130"/>
     </row>
-    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="98" t="s">
         <v>190</v>
       </c>
@@ -5772,7 +5761,7 @@
       <c r="C23" s="130"/>
       <c r="D23" s="130"/>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="98" t="s">
         <v>192</v>
       </c>
@@ -5782,31 +5771,31 @@
       <c r="C24" s="130"/>
       <c r="D24" s="130"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="95"/>
       <c r="B25" s="128"/>
       <c r="C25" s="128"/>
       <c r="D25" s="128"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="95"/>
       <c r="B26" s="128"/>
       <c r="C26" s="128"/>
       <c r="D26" s="128"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="95"/>
       <c r="B27" s="128"/>
       <c r="C27" s="128"/>
       <c r="D27" s="128"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="95"/>
       <c r="B28" s="128"/>
       <c r="C28" s="128"/>
       <c r="D28" s="128"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="95"/>
       <c r="B29" s="128"/>
       <c r="C29" s="128"/>
@@ -5847,21 +5836,21 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="35"/>
-    <col min="2" max="2" width="8.1796875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="61.54296875" style="23" customWidth="1"/>
-    <col min="4" max="6" width="11.453125" style="23"/>
+    <col min="1" max="1" width="11.42578125" style="35"/>
+    <col min="2" max="2" width="8.140625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" style="23" customWidth="1"/>
+    <col min="4" max="6" width="11.42578125" style="23"/>
     <col min="7" max="7" width="60" style="23" customWidth="1"/>
-    <col min="8" max="1024" width="11.453125" style="23"/>
+    <col min="8" max="1024" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="124" t="s">
         <v>215</v>
       </c>
@@ -5873,11 +5862,11 @@
       <c r="F1" s="124"/>
       <c r="G1" s="124"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
     </row>
-    <row r="3" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>194</v>
       </c>
@@ -5897,7 +5886,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>45188</v>
       </c>
@@ -5917,7 +5906,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>45236</v>
       </c>
@@ -5937,7 +5926,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>45236</v>
       </c>
@@ -5957,7 +5946,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>45236</v>
       </c>
@@ -5977,7 +5966,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>45243</v>
       </c>
@@ -5997,7 +5986,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>45243</v>
       </c>
@@ -6017,7 +6006,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>45243</v>
       </c>
@@ -6037,7 +6026,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>45250</v>
       </c>
@@ -6057,7 +6046,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>45250</v>
       </c>
@@ -6077,7 +6066,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>45257</v>
       </c>
@@ -6097,12 +6086,12 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>45257</v>
       </c>
       <c r="B14" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>231</v>
@@ -6111,7 +6100,7 @@
       <c r="F14" s="41"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="41"/>
       <c r="C15" s="2"/>
@@ -6119,7 +6108,7 @@
       <c r="F15" s="41"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="41"/>
       <c r="C16" s="2"/>
@@ -6127,7 +6116,7 @@
       <c r="F16" s="41"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="41"/>
       <c r="C17" s="2"/>
@@ -6135,7 +6124,7 @@
       <c r="F17" s="41"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="41"/>
       <c r="C18" s="2"/>
@@ -6143,7 +6132,7 @@
       <c r="F18" s="41"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="41"/>
       <c r="C19" s="2"/>
@@ -6151,7 +6140,7 @@
       <c r="F19" s="41"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="41"/>
       <c r="C20" s="2"/>
@@ -6159,7 +6148,7 @@
       <c r="F20" s="41"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
       <c r="C21" s="2"/>
@@ -6167,7 +6156,7 @@
       <c r="F21" s="41"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
       <c r="B22" s="41"/>
       <c r="C22" s="2"/>
@@ -6175,7 +6164,7 @@
       <c r="F22" s="41"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
       <c r="C23" s="2"/>
@@ -6183,7 +6172,7 @@
       <c r="F23" s="41"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
       <c r="B24" s="41"/>
       <c r="C24" s="2"/>
@@ -6191,7 +6180,7 @@
       <c r="F24" s="41"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="2"/>
@@ -6199,7 +6188,7 @@
       <c r="F25" s="41"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="2"/>
@@ -6207,7 +6196,7 @@
       <c r="F26" s="41"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="2"/>
@@ -6215,7 +6204,7 @@
       <c r="F27" s="41"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
       <c r="B28" s="41"/>
       <c r="C28" s="2"/>
@@ -6223,7 +6212,7 @@
       <c r="F28" s="41"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="41"/>
       <c r="C29" s="2"/>
@@ -6231,7 +6220,7 @@
       <c r="F29" s="41"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="41"/>
       <c r="B30" s="41"/>
       <c r="C30" s="2"/>
@@ -6239,7 +6228,7 @@
       <c r="F30" s="41"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="41"/>
       <c r="B31" s="41"/>
       <c r="C31" s="2"/>
@@ -6247,7 +6236,7 @@
       <c r="F31" s="41"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
       <c r="B32" s="41"/>
       <c r="C32" s="2"/>
@@ -6255,7 +6244,7 @@
       <c r="F32" s="41"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
       <c r="C33" s="24"/>

</xml_diff>